<commit_message>
add xuất nhập logic, tiếp tục với mapping
</commit_message>
<xml_diff>
--- a/bang_ke/bly/Nova/mapping.xlsx
+++ b/bang_ke/bly/Nova/mapping.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Tools\bang_ke\bly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Tools\bang_ke\bly\Nova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17716EC-58CF-4A9D-AE3F-D4A6FACB1A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8316EF-2560-4952-A364-DBFEC9253CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12384" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nova Nhập" sheetId="1" r:id="rId1"/>
     <sheet name="Phụ Phí Nhập" sheetId="3" r:id="rId2"/>
-    <sheet name="Nova Xuất" sheetId="2" r:id="rId3"/>
-    <sheet name="xuất" sheetId="5" r:id="rId4"/>
-    <sheet name="nhập" sheetId="4" r:id="rId5"/>
+    <sheet name="nhập" sheetId="4" r:id="rId3"/>
+    <sheet name="Nova Xuất" sheetId="2" r:id="rId4"/>
+    <sheet name="Phụ Phí Xuất" sheetId="6" r:id="rId5"/>
+    <sheet name="xuất" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="65">
   <si>
     <t>File Theo Dõi</t>
   </si>
@@ -386,6 +387,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -393,12 +400,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -685,7 +686,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -971,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -989,11 +990,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
@@ -1372,583 +1373,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E74A2A-EDEF-409E-96F2-A4FAC7649A80}">
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="40.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EAFB3DE-3B9E-435A-9250-4E09B7BAA52F}">
-  <dimension ref="A1:C39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="40.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E74A2A-EDEF-409E-96F2-A4FAC7649A80}">
-  <dimension ref="A1:C39"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1971,145 +1399,145 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="3"/>
@@ -2227,4 +1655,981 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="40.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08943AFA-2AA7-4D7B-A949-F5B7BEB4174D}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29" style="5" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="5"/>
+    <col min="7" max="16384" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EAFB3DE-3B9E-435A-9250-4E09B7BAA52F}">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="40.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>